<commit_message>
update solution space size SAD to code in result files
</commit_message>
<xml_diff>
--- a/results/ArDoCode.xlsx
+++ b/results/ArDoCode.xlsx
@@ -220,12 +220,12 @@
   <dimension ref="B3:H10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="1" sqref="C4 E4"/>
+      <selection pane="topLeft" activeCell="E4" activeCellId="1" sqref="C13:C17 E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.84765625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.859375" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="8.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="8.72"/>
@@ -448,12 +448,12 @@
   <dimension ref="B2:E17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13:C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.84765625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.859375" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.28"/>
   </cols>
   <sheetData>
@@ -565,12 +565,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="0" t="s">
         <v>7</v>
       </c>
       <c r="C13" s="0" t="n">
-        <v>47600</v>
+        <v>46495</v>
       </c>
       <c r="D13" s="0" t="n">
         <v>1020</v>
@@ -579,12 +579,12 @@
         <v>13440</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
         <v>8</v>
       </c>
       <c r="C14" s="0" t="n">
-        <v>26000</v>
+        <v>25727</v>
       </c>
       <c r="D14" s="0" t="n">
         <v>78</v>
@@ -593,7 +593,7 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
         <v>9</v>
       </c>
@@ -607,12 +607,12 @@
         <v>2231</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
         <v>10</v>
       </c>
       <c r="C16" s="0" t="n">
-        <v>165330</v>
+        <v>164736</v>
       </c>
       <c r="D16" s="0" t="n">
         <v>1584</v>
@@ -621,7 +621,7 @@
         <v>13360</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="0" t="s">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
update solution space size SAM to code in result files
</commit_message>
<xml_diff>
--- a/results/ArDoCode.xlsx
+++ b/results/ArDoCode.xlsx
@@ -220,10 +220,10 @@
   <dimension ref="B3:H10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="1" sqref="C13:C17 E4"/>
+      <selection pane="topLeft" activeCell="E4" activeCellId="1" sqref="E13:E17 E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.859375" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.8671875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.18"/>
@@ -448,10 +448,10 @@
   <dimension ref="B2:E17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13:C17"/>
+      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13:E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.859375" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.8671875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.28"/>
@@ -576,7 +576,7 @@
         <v>1020</v>
       </c>
       <c r="E13" s="0" t="n">
-        <v>13440</v>
+        <v>13128</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -590,7 +590,7 @@
         <v>78</v>
       </c>
       <c r="E14" s="0" t="n">
-        <v>12000</v>
+        <v>11874</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -618,7 +618,7 @@
         <v>1584</v>
       </c>
       <c r="E16" s="0" t="n">
-        <v>13360</v>
+        <v>13312</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>